<commit_message>
Project 3 is done
</commit_message>
<xml_diff>
--- a/Evolutionary_Sequence_of_CPUs/6-Vertebrate/vertebrate_microcode_fsm.xlsx
+++ b/Evolutionary_Sequence_of_CPUs/6-Vertebrate/vertebrate_microcode_fsm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsan\projects\school\CSE4117-Microprocessors\Evolutionary_Sequence_of_CPUs\6-Vertebrate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A244B63D-38B3-4D44-B648-38D2855BA56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713BEDA8-FE09-4268-B19D-9D3F55B283D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
   <si>
     <t>Address</t>
   </si>
@@ -227,9 +227,6 @@
     <t>STI</t>
   </si>
   <si>
-    <t>12-bit Address Bus Vertebrate CPU Microcode</t>
-  </si>
-  <si>
     <t>HEX CODE</t>
   </si>
   <si>
@@ -306,6 +303,21 @@
   </si>
   <si>
     <t>opcode:1110</t>
+  </si>
+  <si>
+    <t>0x5</t>
+  </si>
+  <si>
+    <t>16-bit Address Bus Vertebrate CPU Microcode</t>
+  </si>
+  <si>
+    <t>RET3</t>
+  </si>
+  <si>
+    <t>0x16</t>
+  </si>
+  <si>
+    <t>0x1f</t>
   </si>
 </sst>
 </file>
@@ -430,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -500,6 +512,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,6 +544,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -846,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C1B6C-1DD3-447E-A634-9FBDC6E555DB}">
   <dimension ref="C1:AW34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,86 +873,86 @@
     <col min="5" max="24" width="4.140625" customWidth="1"/>
     <col min="25" max="25" width="7.5703125" customWidth="1"/>
     <col min="26" max="26" width="4.140625" customWidth="1"/>
-    <col min="27" max="27" width="32.85546875" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="5" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" customWidth="1"/>
     <col min="29" max="29" width="11.5703125" customWidth="1"/>
     <col min="30" max="43" width="4.140625" customWidth="1"/>
     <col min="44" max="44" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
     </row>
     <row r="2" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
     </row>
     <row r="3" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="34"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
     </row>
     <row r="6" spans="3:49" x14ac:dyDescent="0.25">
       <c r="AA6" s="14"/>
@@ -987,38 +1005,38 @@
       <c r="AW7" s="16"/>
     </row>
     <row r="8" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="D8" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
+      <c r="D8" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
-      <c r="AC8" s="32"/>
-      <c r="AD8" s="32"/>
-      <c r="AE8" s="32"/>
-      <c r="AF8" s="32"/>
-      <c r="AG8" s="32"/>
-      <c r="AH8" s="32"/>
-      <c r="AI8" s="32"/>
-      <c r="AJ8" s="32"/>
-      <c r="AK8" s="32"/>
-      <c r="AL8" s="32"/>
-      <c r="AM8" s="32"/>
+      <c r="AC8" s="33"/>
+      <c r="AD8" s="33"/>
+      <c r="AE8" s="33"/>
+      <c r="AF8" s="33"/>
+      <c r="AG8" s="33"/>
+      <c r="AH8" s="33"/>
+      <c r="AI8" s="33"/>
+      <c r="AJ8" s="33"/>
+      <c r="AK8" s="33"/>
+      <c r="AL8" s="33"/>
+      <c r="AM8" s="33"/>
       <c r="AN8" s="14"/>
       <c r="AO8" s="14"/>
       <c r="AP8" s="14"/>
@@ -1035,25 +1053,25 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>1</v>
@@ -1128,13 +1146,13 @@
         <v>18</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>47</v>
@@ -1143,10 +1161,10 @@
         <v>55</v>
       </c>
       <c r="K10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>19</v>
@@ -1190,7 +1208,7 @@
       <c r="AA10" s="14"/>
       <c r="AB10" s="14"/>
       <c r="AC10" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AD10" s="17"/>
       <c r="AE10" s="18"/>
@@ -1247,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="Z11" s="6"/>
       <c r="AA11" s="23" t="str" cm="1">
@@ -1260,7 +1278,7 @@
       </c>
       <c r="AC11" s="24" t="str">
         <f>DEC2HEX(_xlfn.BITLSHIFT(AB11,5) + HEX2DEC(MID(Y11,3,2)))</f>
-        <v>1001020</v>
+        <v>100103F</v>
       </c>
       <c r="AD11" s="15"/>
       <c r="AE11" s="15"/>
@@ -1325,11 +1343,11 @@
         <v>00000000000010010100</v>
       </c>
       <c r="AB12" s="23">
-        <f t="shared" ref="AB12:AB32" si="0">HEX2DEC(BIN2HEX(MID(AA12,1,4))&amp;  BIN2HEX(MID(AA12,5,4))&amp;  BIN2HEX(MID(AA12,9,4))&amp;  BIN2HEX(MID(AA12,13,4)) &amp; BIN2HEX(MID(AA12,17,4)))</f>
+        <f t="shared" ref="AB12:AB33" si="0">HEX2DEC(BIN2HEX(MID(AA12,1,4))&amp;  BIN2HEX(MID(AA12,5,4))&amp;  BIN2HEX(MID(AA12,9,4))&amp;  BIN2HEX(MID(AA12,13,4)) &amp; BIN2HEX(MID(AA12,17,4)))</f>
         <v>148</v>
       </c>
       <c r="AC12" s="30" t="str">
-        <f t="shared" ref="AC12:AC32" si="1">DEC2HEX(_xlfn.BITLSHIFT(AB12,5) + HEX2DEC(MID(Y12,3,2)))</f>
+        <f t="shared" ref="AC12:AC33" si="1">DEC2HEX(_xlfn.BITLSHIFT(AB12,5) + HEX2DEC(MID(Y12,3,2)))</f>
         <v>1280</v>
       </c>
       <c r="AD12" s="15"/>
@@ -1510,7 +1528,9 @@
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
       <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
+      <c r="Q15" s="20">
+        <v>1</v>
+      </c>
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
       <c r="T15" s="20"/>
@@ -1524,15 +1544,15 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="23" t="str" cm="1">
         <f t="array" ref="AA15">_xlfn.TEXTJOIN("",TRUE,IF(E15:X15="",0,E15:X15))</f>
-        <v>00000000000000000000</v>
+        <v>00000000000010000000</v>
       </c>
       <c r="AB15" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="AC15" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AD15" s="15"/>
       <c r="AE15" s="15"/>
@@ -1851,7 +1871,7 @@
       <c r="W20" s="21"/>
       <c r="X20" s="21"/>
       <c r="Y20" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA20" s="23" t="str" cm="1">
         <f t="array" ref="AA20">_xlfn.TEXTJOIN("",TRUE,IF(E20:X20="",0,E20:X20))</f>
@@ -1908,9 +1928,7 @@
       <c r="O21" s="20">
         <v>1</v>
       </c>
-      <c r="P21" s="20">
-        <v>1</v>
-      </c>
+      <c r="P21" s="20"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="20">
         <v>1</v>
@@ -1918,25 +1936,27 @@
       <c r="S21" s="20"/>
       <c r="T21" s="20"/>
       <c r="U21" s="20"/>
-      <c r="V21" s="20"/>
+      <c r="V21" s="20">
+        <v>1</v>
+      </c>
       <c r="W21" s="20">
         <v>1</v>
       </c>
       <c r="X21" s="20"/>
       <c r="Y21" s="2" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="AA21" s="23" t="str" cm="1">
         <f t="array" ref="AA21">_xlfn.TEXTJOIN("",TRUE,IF(E21:X21="",0,E21:X21))</f>
-        <v>00000001001101000010</v>
+        <v>00000001001001000110</v>
       </c>
       <c r="AB21" s="23">
         <f t="shared" si="0"/>
-        <v>4930</v>
+        <v>4678</v>
       </c>
       <c r="AC21" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>26840</v>
+        <v>248C5</v>
       </c>
       <c r="AD21" s="15"/>
       <c r="AE21" s="15"/>
@@ -1989,7 +2009,7 @@
       <c r="W22" s="21"/>
       <c r="X22" s="21"/>
       <c r="Y22" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA22" s="23" t="str" cm="1">
         <f t="array" ref="AA22">_xlfn.TEXTJOIN("",TRUE,IF(E22:X22="",0,E22:X22))</f>
@@ -2046,17 +2066,11 @@
       <c r="O23" s="20"/>
       <c r="P23" s="20"/>
       <c r="Q23" s="20"/>
-      <c r="R23" s="20">
-        <v>1</v>
-      </c>
+      <c r="R23" s="20"/>
       <c r="S23" s="20"/>
-      <c r="T23" s="20">
-        <v>1</v>
-      </c>
+      <c r="T23" s="20"/>
       <c r="U23" s="20"/>
-      <c r="V23" s="20">
-        <v>1</v>
-      </c>
+      <c r="V23" s="20"/>
       <c r="W23" s="20"/>
       <c r="X23" s="20"/>
       <c r="Y23" s="2" t="s">
@@ -2064,15 +2078,15 @@
       </c>
       <c r="AA23" s="23" t="str" cm="1">
         <f t="array" ref="AA23">_xlfn.TEXTJOIN("",TRUE,IF(E23:X23="",0,E23:X23))</f>
-        <v>00000100000001010100</v>
+        <v>00000100000000000000</v>
       </c>
       <c r="AB23" s="23">
         <f t="shared" si="0"/>
-        <v>16468</v>
+        <v>16384</v>
       </c>
       <c r="AC23" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>80A80</v>
+        <v>80000</v>
       </c>
       <c r="AD23" s="15"/>
       <c r="AE23" s="15"/>
@@ -2112,24 +2126,16 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
-      <c r="M24" s="21">
-        <v>1</v>
-      </c>
+      <c r="M24" s="21"/>
       <c r="N24" s="21"/>
       <c r="O24" s="21"/>
-      <c r="P24" s="21">
-        <v>1</v>
-      </c>
+      <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
-      <c r="R24" s="21">
-        <v>1</v>
-      </c>
+      <c r="R24" s="21"/>
       <c r="S24" s="21"/>
       <c r="T24" s="21"/>
       <c r="U24" s="21"/>
-      <c r="V24" s="21">
-        <v>1</v>
-      </c>
+      <c r="V24" s="21"/>
       <c r="W24" s="21"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="5" t="s">
@@ -2137,15 +2143,15 @@
       </c>
       <c r="AA24" s="23" t="str" cm="1">
         <f t="array" ref="AA24">_xlfn.TEXTJOIN("",TRUE,IF(E24:X24="",0,E24:X24))</f>
-        <v>00001000100101000100</v>
+        <v>00001000000000000000</v>
       </c>
       <c r="AB24" s="23">
         <f t="shared" si="0"/>
-        <v>35140</v>
+        <v>32768</v>
       </c>
       <c r="AC24" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>112880</v>
+        <v>100000</v>
       </c>
       <c r="AD24" s="15"/>
       <c r="AE24" s="15"/>
@@ -2173,7 +2179,7 @@
         <v>48</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
@@ -2198,7 +2204,7 @@
       <c r="W25" s="20"/>
       <c r="X25" s="20"/>
       <c r="Y25" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA25" s="23" t="str" cm="1">
         <f t="array" ref="AA25">_xlfn.TEXTJOIN("",TRUE,IF(E25:X25="",0,E25:X25))</f>
@@ -2238,7 +2244,7 @@
         <v>49</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -2248,24 +2254,18 @@
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
-      <c r="M26" s="22">
-        <v>1</v>
-      </c>
+      <c r="M26" s="22"/>
       <c r="N26" s="22">
         <v>1</v>
       </c>
       <c r="O26" s="22"/>
-      <c r="P26" s="22">
-        <v>1</v>
-      </c>
+      <c r="P26" s="22"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="22">
         <v>1</v>
       </c>
       <c r="S26" s="22"/>
-      <c r="T26" s="22">
-        <v>1</v>
-      </c>
+      <c r="T26" s="22"/>
       <c r="U26" s="22"/>
       <c r="V26" s="22">
         <v>1</v>
@@ -2273,19 +2273,19 @@
       <c r="W26" s="22"/>
       <c r="X26" s="22"/>
       <c r="Y26" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA26" s="23" t="str" cm="1">
         <f t="array" ref="AA26">_xlfn.TEXTJOIN("",TRUE,IF(E26:X26="",0,E26:X26))</f>
-        <v>00000000110101010100</v>
+        <v>00000000010001000100</v>
       </c>
       <c r="AB26" s="23">
         <f t="shared" si="0"/>
-        <v>3412</v>
+        <v>1092</v>
       </c>
       <c r="AC26" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>1AA90</v>
+        <v>8890</v>
       </c>
       <c r="AD26" s="15"/>
       <c r="AE26" s="15"/>
@@ -2325,10 +2325,14 @@
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
+      <c r="M27" s="20">
+        <v>1</v>
+      </c>
       <c r="N27" s="20"/>
       <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
+      <c r="P27" s="20">
+        <v>1</v>
+      </c>
       <c r="Q27" s="20"/>
       <c r="R27" s="20">
         <v>1</v>
@@ -2344,15 +2348,15 @@
       </c>
       <c r="AA27" s="23" t="str" cm="1">
         <f t="array" ref="AA27">_xlfn.TEXTJOIN("",TRUE,IF(E27:X27="",0,E27:X27))</f>
-        <v>01000000000001000000</v>
+        <v>01000000100101000000</v>
       </c>
       <c r="AB27" s="23">
         <f t="shared" si="0"/>
-        <v>262208</v>
+        <v>264512</v>
       </c>
       <c r="AC27" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>800800</v>
+        <v>812800</v>
       </c>
       <c r="AD27" s="15"/>
       <c r="AE27" s="15"/>
@@ -2399,7 +2403,9 @@
         <v>1</v>
       </c>
       <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
+      <c r="T28" s="21">
+        <v>1</v>
+      </c>
       <c r="U28" s="21"/>
       <c r="V28" s="21">
         <v>1</v>
@@ -2411,15 +2417,15 @@
       </c>
       <c r="AA28" s="23" t="str" cm="1">
         <f t="array" ref="AA28">_xlfn.TEXTJOIN("",TRUE,IF(E28:X28="",0,E28:X28))</f>
-        <v>00000000000001000100</v>
+        <v>00000000000001010100</v>
       </c>
       <c r="AB28" s="23">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="AC28" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>880</v>
+        <v>A80</v>
       </c>
       <c r="AD28" s="15"/>
       <c r="AE28" s="15"/>
@@ -2457,7 +2463,9 @@
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
+      <c r="M29" s="20">
+        <v>1</v>
+      </c>
       <c r="N29" s="20"/>
       <c r="O29" s="20"/>
       <c r="P29" s="20">
@@ -2476,19 +2484,19 @@
       <c r="W29" s="20"/>
       <c r="X29" s="20"/>
       <c r="Y29" s="2" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="AA29" s="23" t="str" cm="1">
         <f t="array" ref="AA29">_xlfn.TEXTJOIN("",TRUE,IF(E29:X29="",0,E29:X29))</f>
-        <v>00000000000101000100</v>
+        <v>00000000100101000100</v>
       </c>
       <c r="AB29" s="23">
         <f t="shared" si="0"/>
-        <v>324</v>
+        <v>2372</v>
       </c>
       <c r="AC29" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>2880</v>
+        <v>12896</v>
       </c>
       <c r="AD29" s="15"/>
       <c r="AE29" s="15"/>
@@ -2532,7 +2540,9 @@
       </c>
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
+      <c r="O30" s="21">
+        <v>1</v>
+      </c>
       <c r="P30" s="21"/>
       <c r="Q30" s="21"/>
       <c r="R30" s="21">
@@ -2547,19 +2557,19 @@
       </c>
       <c r="X30" s="21"/>
       <c r="Y30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA30" s="23" t="str" cm="1">
         <f t="array" ref="AA30">_xlfn.TEXTJOIN("",TRUE,IF(E30:X30="",0,E30:X30))</f>
-        <v>00001001000001000010</v>
+        <v>00001001001001000010</v>
       </c>
       <c r="AB30" s="23">
         <f t="shared" si="0"/>
-        <v>36930</v>
+        <v>37442</v>
       </c>
       <c r="AC30" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>120854</v>
+        <v>124854</v>
       </c>
       <c r="AD30" s="14"/>
       <c r="AE30" s="14"/>
@@ -2620,7 +2630,7 @@
       </c>
       <c r="X31" s="20"/>
       <c r="Y31" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA31" s="23" t="str" cm="1">
         <f t="array" ref="AA31">_xlfn.TEXTJOIN("",TRUE,IF(E31:X31="",0,E31:X31))</f>
@@ -2712,7 +2722,50 @@
       <c r="AV32" s="16"/>
       <c r="AW32" s="16"/>
     </row>
-    <row r="33" spans="44:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C33" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="3">
+        <v>16</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="42">
+        <v>1</v>
+      </c>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA33" s="23" t="str" cm="1">
+        <f t="array" ref="AA33">_xlfn.TEXTJOIN("",TRUE,IF(E33:X33="",0,E33:X33))</f>
+        <v>00000000000010000000</v>
+      </c>
+      <c r="AB33" s="23">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="AC33" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
       <c r="AR33" s="16"/>
       <c r="AS33" s="16"/>
       <c r="AT33" s="16"/>
@@ -2720,7 +2773,7 @@
       <c r="AV33" s="16"/>
       <c r="AW33" s="16"/>
     </row>
-    <row r="34" spans="44:49" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:49" x14ac:dyDescent="0.25">
       <c r="AR34" s="16"/>
       <c r="AS34" s="16"/>
       <c r="AT34" s="16"/>
@@ -2755,24 +2808,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C3" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
+      <c r="C3" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
       <c r="W3" s="26"/>
       <c r="X3" s="26"/>
       <c r="Y3" s="26"/>
@@ -2827,15 +2880,15 @@
       <c r="AL5" s="16"/>
     </row>
     <row r="6" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="38"/>
       <c r="W6" s="26"/>
       <c r="X6" s="26"/>
       <c r="Y6" s="26"/>
@@ -2920,26 +2973,26 @@
       <c r="AL7" s="25"/>
     </row>
     <row r="8" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C8" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="35" t="s">
+      <c r="C8" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="38"/>
       <c r="W8" s="27"/>
       <c r="X8" s="27"/>
       <c r="Y8" s="27"/>
@@ -3034,15 +3087,15 @@
       <c r="AL12" s="16"/>
     </row>
     <row r="13" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
       <c r="W13" s="26"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
@@ -3127,26 +3180,26 @@
       <c r="AL14" s="25"/>
     </row>
     <row r="15" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C15" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="35" t="s">
+      <c r="C15" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="38"/>
       <c r="W15" s="27"/>
       <c r="X15" s="27"/>
       <c r="Y15" s="27"/>
@@ -3241,15 +3294,15 @@
       <c r="AL19" s="16"/>
     </row>
     <row r="20" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C20" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="C20" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
       <c r="W20" s="26"/>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -3334,23 +3387,23 @@
       <c r="AL21" s="25"/>
     </row>
     <row r="22" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C22" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="35" t="s">
+      <c r="C22" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
       <c r="P22" s="29">
         <v>1</v>
       </c>

</xml_diff>